<commit_message>
Fixed the excel table with actual score formulas
</commit_message>
<xml_diff>
--- a/Нови изисквания за курса от Крушков/FN0328009.xlsx
+++ b/Нови изисквания за курса от Крушков/FN0328009.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luben\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
@@ -22,17 +17,17 @@
     <definedName name="ColumnTitle2">Домашни[[#Headers],[Дата]]</definedName>
     <definedName name="ColumnTitle3">#REF!</definedName>
     <definedName name="CurrentShit">Income[]</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Начало!$16:$16</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Самостоятелна работа'!$6:$6</definedName>
     <definedName name="Total_Homeworks_Points">Начало!$C$8</definedName>
     <definedName name="Total_Monthly_Expenses">Начало!#REF!</definedName>
     <definedName name="Total_Monthly_Savings">Начало!$C$8</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Начало!$16:$16</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Самостоятелна работа'!$6:$6</definedName>
     <definedName name="Семестриален_изпит">Начало!$C$10</definedName>
-    <definedName name="СР">'Самостоятелна работа'!$G$13</definedName>
+    <definedName name="СР">'Самостоятелна работа'!$G$20</definedName>
     <definedName name="Текущ_Контрол">Начало!$C$6</definedName>
     <definedName name="ТекущКонтрол">Начало!$C$6</definedName>
   </definedNames>
-  <calcPr calcId="162913" calcMode="autoNoTable"/>
+  <calcPr calcId="145621" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -42,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>CHART DATA</t>
   </si>
@@ -86,9 +81,6 @@
     <t>Работещи задачи</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Предадени домашни, присъствия, презентации и др.</t>
   </si>
   <si>
@@ -116,18 +108,9 @@
     <t>* Макс. точки от домашни : 40 (8 упражнения за семестър * 5 точки за домашно);</t>
   </si>
   <si>
-    <t>* При натрупан максимален брой точки (95) се раздават допълнителни + 5 бонус точки</t>
-  </si>
-  <si>
-    <t>* Макс. точки от презентации : 15/30 (по 15 точки за всяка презентация. Макс. презентации за семестър : 2 !при положение, че има свободни слотове);</t>
-  </si>
-  <si>
     <t>Точки :</t>
   </si>
   <si>
-    <t>СР (Самостоятелна работа) = СР * 0.2 :</t>
-  </si>
-  <si>
     <t>ТК (Текущ контрол) = (ТК1 + ТК2) * 0.2</t>
   </si>
   <si>
@@ -147,19 +130,31 @@
   </si>
   <si>
     <t>ТК</t>
+  </si>
+  <si>
+    <t>Бонус точки:</t>
+  </si>
+  <si>
+    <t>* Макс. точки за презентации : 20 точки;</t>
+  </si>
+  <si>
+    <t>* При натрупан максимален брой точки (100) се раздават допълнителни + 20 бонус точки;</t>
+  </si>
+  <si>
+    <t>СР (Самостоятелна работа) = (СР / 2) * 0.2 :</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="26" x14ac:knownFonts="1">
+  <fonts count="29" x14ac:knownFonts="1">
     <font>
       <b/>
       <sz val="12"/>
@@ -346,8 +341,30 @@
       <color theme="3" tint="0.24994659260841701"/>
       <name val="Constantia"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="0.24994659260841701"/>
+      <name val="Constantia"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Constantia"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="3" tint="0.24994659260841701"/>
+      <name val="Constantia"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +384,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -413,22 +436,22 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left"/>
@@ -490,41 +513,41 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="4" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="20" fillId="4" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
@@ -560,54 +583,86 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="17" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="17" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="27" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="13">
     <cellStyle name="% Income Spent" xfId="6"/>
-    <cellStyle name="Accent6" xfId="12" builtinId="49"/>
     <cellStyle name="Amount" xfId="7"/>
-    <cellStyle name="Currency" xfId="8" builtinId="4"/>
-    <cellStyle name="Good" xfId="9" builtinId="26"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Note" xfId="10" builtinId="10"/>
     <cellStyle name="Summary" xfId="5"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="11" builtinId="25"/>
+    <cellStyle name="Акцент6" xfId="12" builtinId="49"/>
+    <cellStyle name="Бележка" xfId="10" builtinId="10"/>
+    <cellStyle name="Валута" xfId="8" builtinId="4"/>
+    <cellStyle name="Добър" xfId="9" builtinId="26"/>
+    <cellStyle name="Заглавие" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Заглавие 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Заглавие 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Заглавие 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Нормален" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Сума" xfId="11" builtinId="25"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -679,7 +734,7 @@
         <name val="Constantia"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -766,11 +821,6 @@
       </font>
     </dxf>
     <dxf>
-      <font>
-        <color theme="5" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
       <border>
         <top style="thin">
           <color theme="2" tint="-0.24994659260841701"/>
@@ -822,7 +872,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="B16:C22" headerRowDxfId="12" dataDxfId="11" totalsRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="B16:C22" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
   <autoFilter ref="B16:C22">
     <filterColumn colId="0">
       <filters>
@@ -832,8 +882,8 @@
     </filterColumn>
   </autoFilter>
   <tableColumns count="2">
-    <tableColumn id="1" name="Наименование" totalsRowLabel="Total" dataDxfId="9"/>
-    <tableColumn id="2" name="Оценка" totalsRowFunction="sum" dataDxfId="8" dataCellStyle="Amount"/>
+    <tableColumn id="1" name="Наименование" totalsRowLabel="Total" dataDxfId="10"/>
+    <tableColumn id="2" name="Оценка" totalsRowFunction="sum" dataDxfId="9" dataCellStyle="Amount"/>
   </tableColumns>
   <tableStyleInfo name="BudgetTable" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -845,15 +895,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Домашни" displayName="Домашни" ref="B6:G12" totalsRowShown="0" headerRowDxfId="7" dataDxfId="6">
-  <autoFilter ref="B6:G12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Домашни" displayName="Домашни" ref="B6:G18" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="B6:G18"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Дата" dataDxfId="5"/>
-    <tableColumn id="5" name="Присъствие на упражнения" dataDxfId="4"/>
-    <tableColumn id="6" name="Презентация" dataDxfId="3"/>
-    <tableColumn id="3" name="Именоване на проект" dataDxfId="2"/>
-    <tableColumn id="4" name="Работещи задачи" dataDxfId="1"/>
-    <tableColumn id="2" name="Точки" dataDxfId="0" dataCellStyle="Amount"/>
+    <tableColumn id="1" name="Дата" dataDxfId="6"/>
+    <tableColumn id="5" name="Присъствие на упражнения" dataDxfId="5"/>
+    <tableColumn id="6" name="Презентация" dataDxfId="4"/>
+    <tableColumn id="3" name="Именоване на проект" dataDxfId="3"/>
+    <tableColumn id="4" name="Работещи задачи" dataDxfId="2"/>
+    <tableColumn id="2" name="Точки" dataDxfId="1" dataCellStyle="Amount"/>
   </tableColumns>
   <tableStyleInfo name="BudgetTable" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
   <extLst>
@@ -1119,7 +1169,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1133,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1146,20 +1196,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
+      <c r="A1" s="51" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="51" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -1178,7 +1228,7 @@
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="40" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -1186,7 +1236,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="12">
         <f>C20</f>
-        <v>2</v>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.5">
@@ -1195,7 +1245,7 @@
         <v>11</v>
       </c>
       <c r="C7" s="40" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -1203,17 +1253,17 @@
       <c r="B8" s="3"/>
       <c r="C8" s="12">
         <f>[0]!СР</f>
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="3"/>
       <c r="B9" s="16">
         <f>C12/6</f>
-        <v>1.1433333333333333</v>
+        <v>1</v>
       </c>
       <c r="C9" s="40" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.35">
@@ -1236,7 +1286,7 @@
       <c r="B12" s="3"/>
       <c r="C12" s="39">
         <f>Текущ_Контрол+Total_Homeworks_Points+Семестриален_изпит</f>
-        <v>6.8599999999999994</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -1268,7 +1318,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
@@ -1277,13 +1327,13 @@
         <v>5</v>
       </c>
       <c r="C18" s="42">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="45" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C19" s="43">
         <v>6</v>
@@ -1292,17 +1342,17 @@
     <row r="20" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="46" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C20" s="44">
-        <f>SUM(C17:C18)*(2/10)</f>
-        <v>2</v>
+        <f>SUM(C17:C18)/2*(2/10)</f>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="47" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C21" s="44">
         <f>C19*(6/10)</f>
@@ -1311,8 +1361,8 @@
     </row>
     <row r="22" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
-      <c r="B22" s="58"/>
-      <c r="C22" s="59"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1364,10 +1414,10 @@
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M20"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A7" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1382,27 +1432,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="35.25" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="52" t="str">
+      <c r="A1" s="59" t="str">
         <f>BudgetTitle</f>
         <v>Фак.№032800910</v>
       </c>
-      <c r="B1" s="52"/>
-      <c r="C1" s="52"/>
-      <c r="D1" s="52"/>
-      <c r="E1" s="52"/>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="59"/>
+      <c r="G1" s="59"/>
     </row>
     <row r="2" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
+      <c r="A2" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="25"/>
@@ -1415,14 +1465,14 @@
     <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="55" t="s">
+      <c r="C4" s="54" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="55"/>
+      <c r="E4" s="56" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="56"/>
-      <c r="E4" s="57" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="57"/>
+      <c r="F4" s="56"/>
     </row>
     <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1438,10 +1488,10 @@
         <v>10</v>
       </c>
       <c r="C6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="17" t="s">
         <v>16</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>17</v>
       </c>
       <c r="E6" s="17" t="s">
         <v>12</v>
@@ -1464,14 +1514,15 @@
       <c r="D7" s="17">
         <v>0</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>14</v>
+      <c r="E7" s="17">
+        <v>1</v>
       </c>
       <c r="F7" s="17">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G7" s="20">
-        <v>7</v>
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1483,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="17">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
@@ -1492,7 +1543,8 @@
         <v>4</v>
       </c>
       <c r="G8" s="20">
-        <v>25</v>
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1504,161 +1556,295 @@
         <v>5</v>
       </c>
       <c r="D9" s="17">
-        <v>15</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>14</v>
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
       </c>
       <c r="F9" s="17">
         <v>4</v>
       </c>
-      <c r="G9" s="21">
-        <v>24</v>
+      <c r="G9" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="33">
+      <c r="B10" s="61">
         <v>43025</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="60">
         <v>5</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="60">
         <v>0</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="17">
-        <v>2</v>
-      </c>
-      <c r="G10" s="21">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11"/>
-      <c r="B11" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="36"/>
-      <c r="F11" s="36"/>
-      <c r="G11" s="37">
-        <f>SUM(G7:G10)</f>
-        <v>63</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11"/>
-      <c r="K11"/>
-      <c r="L11"/>
-      <c r="M11"/>
-    </row>
-    <row r="12" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12"/>
-      <c r="B12" s="33"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
-      <c r="G12" s="21"/>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12"/>
-      <c r="K12"/>
-      <c r="L12"/>
-      <c r="M12"/>
-    </row>
-    <row r="13" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="60">
+        <v>1</v>
+      </c>
+      <c r="F10" s="60">
+        <v>4</v>
+      </c>
+      <c r="G10" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="3"/>
+      <c r="B11" s="61">
+        <v>43039</v>
+      </c>
+      <c r="C11" s="60">
+        <v>5</v>
+      </c>
+      <c r="D11" s="60">
+        <v>0</v>
+      </c>
+      <c r="E11" s="60">
+        <v>1</v>
+      </c>
+      <c r="F11" s="60">
+        <v>4</v>
+      </c>
+      <c r="G11" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" s="61">
+        <v>43046</v>
+      </c>
+      <c r="C12" s="60">
+        <v>5</v>
+      </c>
+      <c r="D12" s="60">
+        <v>0</v>
+      </c>
+      <c r="E12" s="60">
+        <v>1</v>
+      </c>
+      <c r="F12" s="60">
+        <v>4</v>
+      </c>
+      <c r="G12" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="50" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" s="50"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="31">
-        <f>SUM(G7:G10)*(2/100)</f>
-        <v>1.26</v>
-      </c>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-    </row>
-    <row r="14" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="29"/>
-    </row>
-    <row r="15" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="27" t="s">
+      <c r="B13" s="61">
+        <v>43053</v>
+      </c>
+      <c r="C13" s="60">
+        <v>5</v>
+      </c>
+      <c r="D13" s="60">
+        <v>0</v>
+      </c>
+      <c r="E13" s="60">
+        <v>1</v>
+      </c>
+      <c r="F13" s="60">
+        <v>4</v>
+      </c>
+      <c r="G13" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="3"/>
+      <c r="B14" s="33">
+        <v>43060</v>
+      </c>
+      <c r="C14" s="17">
+        <v>5</v>
+      </c>
+      <c r="D14" s="17">
+        <v>0</v>
+      </c>
+      <c r="E14" s="17">
+        <v>1</v>
+      </c>
+      <c r="F14" s="17">
+        <v>4</v>
+      </c>
+      <c r="G14" s="20">
+        <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="67"/>
+      <c r="F15" s="67"/>
+      <c r="G15" s="68"/>
+    </row>
+    <row r="16" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16"/>
+      <c r="B16" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36"/>
+      <c r="E16" s="36"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37">
+        <f>SUM(G7:G14)</f>
+        <v>100</v>
+      </c>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+    </row>
+    <row r="17" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
+      <c r="G17" s="21"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+    </row>
+    <row r="18" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18"/>
+      <c r="B18" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="64"/>
+      <c r="D18" s="64"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="65">
+        <f>IF(G16 = 100,20,0)</f>
         <v>20</v>
       </c>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-    </row>
-    <row r="16" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="53" t="s">
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+    </row>
+    <row r="19" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="62"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+    </row>
+    <row r="20" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="57" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="57"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="31">
+        <f>(SUM(G7:G14) + G18)/2*(2/100)</f>
+        <v>1.2</v>
+      </c>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+    </row>
+    <row r="21" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="29"/>
+    </row>
+    <row r="22" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="26"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+    </row>
+    <row r="23" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="52" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+    </row>
+    <row r="24" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="52" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="52"/>
+      <c r="D24" s="52"/>
+      <c r="E24" s="27"/>
+    </row>
+    <row r="25" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+      <c r="G25" s="52"/>
+    </row>
+    <row r="26" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="53"/>
-    </row>
-    <row r="17" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="53" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="53"/>
-      <c r="E17" s="27"/>
-    </row>
-    <row r="18" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="53"/>
-      <c r="E18" s="53"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-    </row>
-    <row r="19" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="53" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="54"/>
-    </row>
-    <row r="20" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="53" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="54"/>
-      <c r="E20" s="54"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="53"/>
+    </row>
+    <row r="27" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="53"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B25:G25"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B16:E16"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter savings amount in this column" sqref="G6"/>

</xml_diff>

<commit_message>
Updated some calculations in student excel sheet.
</commit_message>
<xml_diff>
--- a/Нови изисквания за курса от Крушков/FN0328009.xlsx
+++ b/Нови изисквания за курса от Крушков/FN0328009.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luben\OneDrive\Plovdiv University\01. Intro To Programming Course\Увод в програмирането C#\Нови изисквания за курса от Крушков\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
@@ -17,17 +22,17 @@
     <definedName name="ColumnTitle2">Домашни[[#Headers],[Дата]]</definedName>
     <definedName name="ColumnTitle3">#REF!</definedName>
     <definedName name="CurrentShit">Income[]</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="0">Начало!$16:$16</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Самостоятелна работа'!$6:$6</definedName>
     <definedName name="Total_Homeworks_Points">Начало!$C$8</definedName>
     <definedName name="Total_Monthly_Expenses">Начало!#REF!</definedName>
     <definedName name="Total_Monthly_Savings">Начало!$C$8</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="0">Начало!$16:$16</definedName>
-    <definedName name="_xlnm.Print_Titles" localSheetId="1">'Самостоятелна работа'!$6:$6</definedName>
     <definedName name="Семестриален_изпит">Начало!$C$10</definedName>
     <definedName name="СР">'Самостоятелна работа'!$G$20</definedName>
     <definedName name="Текущ_Контрол">Начало!$C$6</definedName>
     <definedName name="ТекущКонтрол">Начало!$C$6</definedName>
   </definedNames>
-  <calcPr calcId="145621" calcMode="autoNoTable"/>
+  <calcPr calcId="162913" calcMode="autoNoTable"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>CHART DATA</t>
   </si>
@@ -142,19 +147,22 @@
   </si>
   <si>
     <t>СР (Самостоятелна работа) = (СР / 2) * 0.2 :</t>
+  </si>
+  <si>
+    <t>Курсова работа</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="&quot;$&quot;#,##0"/>
-    <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <b/>
       <sz val="12"/>
@@ -337,12 +345,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3" tint="0.24994659260841701"/>
-      <name val="Constantia"/>
-    </font>
-    <font>
-      <b/>
       <sz val="12"/>
       <color theme="3" tint="0.24994659260841701"/>
       <name val="Constantia"/>
@@ -363,8 +365,37 @@
       <family val="1"/>
       <charset val="204"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Constantia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Constantia"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -392,8 +423,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -427,8 +463,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="13">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyProtection="0">
@@ -436,22 +496,24 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="28" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2">
       <alignment horizontal="left"/>
@@ -513,41 +575,41 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="19" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="20" fillId="4" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="20" fillId="4" borderId="0" xfId="12" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="12" applyFont="1" applyAlignment="1">
@@ -579,21 +641,49 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="14" fillId="0" borderId="0" xfId="8" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="2" fontId="25" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="26" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="26" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="17" fillId="3" borderId="1" xfId="10" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -605,57 +695,35 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="10" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="18" fillId="2" borderId="0" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="27" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="5" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="28" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="28" fillId="0" borderId="0" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="30" fillId="6" borderId="3" xfId="13" applyFont="1"/>
+    <xf numFmtId="2" fontId="30" fillId="6" borderId="3" xfId="13" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="30" fillId="6" borderId="3" xfId="13" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="14" applyFont="1"/>
+    <xf numFmtId="2" fontId="31" fillId="0" borderId="4" xfId="14" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="13">
+  <cellStyles count="15">
     <cellStyle name="% Income Spent" xfId="6"/>
+    <cellStyle name="Accent6" xfId="12" builtinId="49"/>
     <cellStyle name="Amount" xfId="7"/>
+    <cellStyle name="Currency" xfId="8" builtinId="4"/>
+    <cellStyle name="Good" xfId="9" builtinId="26"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="14" builtinId="24"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="10" builtinId="10"/>
+    <cellStyle name="Output" xfId="13" builtinId="21"/>
     <cellStyle name="Summary" xfId="5"/>
-    <cellStyle name="Акцент6" xfId="12" builtinId="49"/>
-    <cellStyle name="Бележка" xfId="10" builtinId="10"/>
-    <cellStyle name="Валута" xfId="8" builtinId="4"/>
-    <cellStyle name="Добър" xfId="9" builtinId="26"/>
-    <cellStyle name="Заглавие" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Заглавие 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Заглавие 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Заглавие 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Нормален" xfId="0" builtinId="0" customBuiltin="1"/>
-    <cellStyle name="Сума" xfId="11" builtinId="25"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="11" builtinId="25"/>
   </cellStyles>
   <dxfs count="18">
     <dxf>
@@ -734,7 +802,7 @@
         <name val="Constantia"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="167" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="166" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -872,8 +940,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="B16:C22" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
-  <autoFilter ref="B16:C22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Income" displayName="Income" ref="B16:C23" headerRowDxfId="13" dataDxfId="12" totalsRowDxfId="11">
+  <autoFilter ref="B16:C23">
     <filterColumn colId="0">
       <filters>
         <filter val="Income Source 1"/>
@@ -1169,7 +1237,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1181,10 +1249,10 @@
     <tabColor theme="4"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1196,20 +1264,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="10" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="57"/>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="57" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
+      <c r="B2" s="57"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7"/>
@@ -1235,7 +1303,7 @@
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="12">
-        <f>C20</f>
+        <f>C19</f>
         <v>1.2000000000000002</v>
       </c>
     </row>
@@ -1298,7 +1366,7 @@
     </row>
     <row r="15" spans="1:4" ht="45" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
-      <c r="B15" s="48" t="s">
+      <c r="B15" s="47" t="s">
         <v>2</v>
       </c>
       <c r="C15" s="14"/>
@@ -1330,39 +1398,45 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
-      <c r="B19" s="45" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="43">
-        <v>6</v>
+      <c r="B19" s="66" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="67">
+        <f>SUM(C17:C18)/2*(2/10)</f>
+        <v>1.2000000000000002</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
-      <c r="B20" s="46" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="44">
-        <f>SUM(C17:C18)/2*(2/10)</f>
-        <v>1.2000000000000002</v>
+      <c r="B20" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="43">
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="3"/>
-      <c r="B21" s="47" t="s">
+      <c r="B21" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="44">
-        <f>C19*(6/10)</f>
+      <c r="C21" s="67">
+        <f>C20*(6/10)</f>
         <v>3.5999999999999996</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="3"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="50"/>
+    <row r="22" spans="1:3" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="B22" s="69" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="70">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="28.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.45">
+      <c r="B23" s="46"/>
+      <c r="C23" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1416,8 +1490,8 @@
   </sheetPr>
   <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:E27"/>
+    <sheetView showGridLines="0" topLeftCell="B7" zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="28.5" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1465,14 +1539,14 @@
     <row r="4" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="23"/>
-      <c r="C4" s="54" t="s">
+      <c r="C4" s="62" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56" t="s">
+      <c r="D4" s="63"/>
+      <c r="E4" s="64" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="56"/>
+      <c r="F4" s="64"/>
     </row>
     <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
@@ -1534,7 +1608,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="17">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="E8" s="17">
         <v>1</v>
@@ -1544,7 +1618,7 @@
       </c>
       <c r="G8" s="20">
         <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
-        <v>30</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
@@ -1571,41 +1645,41 @@
     </row>
     <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
-      <c r="B10" s="61">
+      <c r="B10" s="49">
         <v>43025</v>
       </c>
-      <c r="C10" s="60">
+      <c r="C10" s="48">
         <v>5</v>
       </c>
-      <c r="D10" s="60">
-        <v>0</v>
-      </c>
-      <c r="E10" s="60">
+      <c r="D10" s="48">
+        <v>20</v>
+      </c>
+      <c r="E10" s="48">
         <v>1</v>
       </c>
-      <c r="F10" s="60">
+      <c r="F10" s="48">
         <v>4</v>
       </c>
       <c r="G10" s="20">
         <f>Домашни[[#This Row],[Присъствие на упражнения]]+Домашни[[#This Row],[Презентация]]+Домашни[[#This Row],[Именоване на проект]]+Домашни[[#This Row],[Работещи задачи]]</f>
-        <v>10</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
-      <c r="B11" s="61">
+      <c r="B11" s="49">
         <v>43039</v>
       </c>
-      <c r="C11" s="60">
+      <c r="C11" s="48">
         <v>5</v>
       </c>
-      <c r="D11" s="60">
+      <c r="D11" s="48">
         <v>0</v>
       </c>
-      <c r="E11" s="60">
+      <c r="E11" s="48">
         <v>1</v>
       </c>
-      <c r="F11" s="60">
+      <c r="F11" s="48">
         <v>4</v>
       </c>
       <c r="G11" s="20">
@@ -1615,19 +1689,19 @@
     </row>
     <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3"/>
-      <c r="B12" s="61">
+      <c r="B12" s="49">
         <v>43046</v>
       </c>
-      <c r="C12" s="60">
+      <c r="C12" s="48">
         <v>5</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="48">
         <v>0</v>
       </c>
-      <c r="E12" s="60">
+      <c r="E12" s="48">
         <v>1</v>
       </c>
-      <c r="F12" s="60">
+      <c r="F12" s="48">
         <v>4</v>
       </c>
       <c r="G12" s="20">
@@ -1637,19 +1711,19 @@
     </row>
     <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3"/>
-      <c r="B13" s="61">
+      <c r="B13" s="49">
         <v>43053</v>
       </c>
-      <c r="C13" s="60">
+      <c r="C13" s="48">
         <v>5</v>
       </c>
-      <c r="D13" s="60">
+      <c r="D13" s="48">
         <v>0</v>
       </c>
-      <c r="E13" s="60">
+      <c r="E13" s="48">
         <v>1</v>
       </c>
-      <c r="F13" s="60">
+      <c r="F13" s="48">
         <v>4</v>
       </c>
       <c r="G13" s="20">
@@ -1681,12 +1755,12 @@
     </row>
     <row r="15" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3"/>
-      <c r="B15" s="66"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="67"/>
-      <c r="E15" s="67"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="68"/>
+      <c r="B15" s="54"/>
+      <c r="C15" s="55"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16"/>
@@ -1725,14 +1799,14 @@
     </row>
     <row r="18" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18"/>
-      <c r="B18" s="63" t="s">
+      <c r="B18" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="64"/>
-      <c r="F18" s="64"/>
-      <c r="G18" s="65">
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="53">
         <f>IF(G16 = 100,20,0)</f>
         <v>20</v>
       </c>
@@ -1745,12 +1819,12 @@
     </row>
     <row r="19" spans="1:13" s="28" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19"/>
-      <c r="B19" s="61"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="62"/>
+      <c r="B19" s="49"/>
+      <c r="C19" s="48"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="50"/>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -1760,10 +1834,10 @@
     </row>
     <row r="20" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3"/>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="65" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="57"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
       <c r="F20" s="28"/>
@@ -1793,58 +1867,58 @@
       <c r="G22" s="26"/>
     </row>
     <row r="23" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="60"/>
     </row>
     <row r="24" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="60" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="52"/>
+      <c r="C24" s="60"/>
+      <c r="D24" s="60"/>
       <c r="E24" s="27"/>
     </row>
     <row r="25" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="52"/>
-      <c r="G25" s="52"/>
+      <c r="C25" s="60"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="60"/>
+      <c r="G25" s="60"/>
     </row>
     <row r="26" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="53"/>
-      <c r="D26" s="53"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="61"/>
     </row>
     <row r="27" spans="1:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="52" t="s">
+      <c r="B27" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="53"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="53"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
+      <c r="E27" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="B20:C20"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A1:G1"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B25:G25"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="B20:C20"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter savings amount in this column" sqref="G6"/>

</xml_diff>